<commit_message>
status 2023 10 01
</commit_message>
<xml_diff>
--- a/Izvedbeni plan 23 24.xlsx
+++ b/Izvedbeni plan 23 24.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PREDAVANJA\NapRacOrodja_ULFS\NapRacOr\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCA99647-7E50-4C91-BD5C-D71A49469D7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{689DE4AA-C302-4513-AAA8-865D65EE304D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -563,7 +563,7 @@
   <dimension ref="A1:M18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Revert "status 2023 10 01"
This reverts commit 1da6e493c07fdba44b5dc8646b068df3a689dab3.
</commit_message>
<xml_diff>
--- a/Izvedbeni plan 23 24.xlsx
+++ b/Izvedbeni plan 23 24.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PREDAVANJA\NapRacOrodja_ULFS\NapRacOr\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{689DE4AA-C302-4513-AAA8-865D65EE304D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCA99647-7E50-4C91-BD5C-D71A49469D7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -563,7 +563,7 @@
   <dimension ref="A1:M18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>